<commit_message>
Improve Excel sample data to fit into new editor width.
</commit_message>
<xml_diff>
--- a/docs/sdk/examples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
+++ b/docs/sdk/examples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annatomanek/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IEUser\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22453F2-BB08-41BD-ABF6-4FCB71FA0E32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="24440" windowHeight="13700" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25425" windowHeight="13485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,13 +180,13 @@
     <t>Full Year (unaudited)</t>
   </si>
   <si>
-    <t>2013 (unaudited)</t>
+    <t>2020 (unaudited)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -304,12 +305,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,20 +624,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" style="1" customWidth="1"/>
-    <col min="2" max="8" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="40.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="4" width="7.375" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="7" width="7.375" customWidth="1"/>
+    <col min="8" max="8" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="8" t="s">
         <v>49</v>
@@ -653,13 +659,13 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="C2" s="3">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="D2" s="3">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
@@ -674,185 +680,185 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>52</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>54</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>53</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>45</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>47</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>47</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>